<commit_message>
add mulitple test fixture
</commit_message>
<xml_diff>
--- a/testcases/excel/bigdata-monjingser1.xlsx
+++ b/testcases/excel/bigdata-monjingser1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20295" windowHeight="8370"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20295" windowHeight="8370" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="sample1_test" sheetId="3" r:id="rId1"/>
@@ -1001,7 +1001,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
@@ -1324,7 +1324,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>

</xml_diff>